<commit_message>
Created CRUD for Zone Testing
</commit_message>
<xml_diff>
--- a/DebugFile.xlsx
+++ b/DebugFile.xlsx
@@ -14,39 +14,165 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <x:si>
-    <x:t>asdasd</x:t>
-  </x:si>
-  <x:si>
-    <x:t>asdsad</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10/24/2022 6:56:24 PM</x:t>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+  <x:si>
+    <x:t>ZoneNameUpdated</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ZoneDescriptionUpdated</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10/25/2022 8:21:16 PM</x:t>
   </x:si>
   <x:si>
     <x:t>https://connectedoffice-devicemanagement.azurewebsites.net/images/edit.png</x:t>
   </x:si>
   <x:si>
-    <x:t>https://connectedoffice-devicemanagement.azurewebsites.net/Zones/Edit/0daf896a-b55a-4a67-b5bc-ff747e1b3238</x:t>
+    <x:t>https://connectedoffice-devicemanagement.azurewebsites.net/Zones/Edit/160f93a1-5bf4-4b75-a93c-d774802f59f7</x:t>
   </x:si>
   <x:si>
     <x:t>https://connectedoffice-devicemanagement.azurewebsites.net/images/details.png</x:t>
   </x:si>
   <x:si>
-    <x:t>https://connectedoffice-devicemanagement.azurewebsites.net/Zones/Details/0daf896a-b55a-4a67-b5bc-ff747e1b3238</x:t>
+    <x:t>https://connectedoffice-devicemanagement.azurewebsites.net/Zones/Details/160f93a1-5bf4-4b75-a93c-d774802f59f7</x:t>
   </x:si>
   <x:si>
     <x:t>https://connectedoffice-devicemanagement.azurewebsites.net/images/delete.png</x:t>
   </x:si>
   <x:si>
-    <x:t>https://connectedoffice-devicemanagement.azurewebsites.net/Zones/Delete/0daf896a-b55a-4a67-b5bc-ff747e1b3238</x:t>
+    <x:t>https://connectedoffice-devicemanagement.azurewebsites.net/Zones/Delete/160f93a1-5bf4-4b75-a93c-d774802f59f7</x:t>
   </x:si>
   <x:si>
     <x:t>https://connectedoffice-devicemanagement.azurewebsites.net/Devices/Details/6c8c8366-a8dc-4ed1-82a2-f2ef67cd97a5</x:t>
   </x:si>
   <x:si>
     <x:t>https://connectedoffice-devicemanagement.azurewebsites.net/Devices/Delete/6c8c8366-a8dc-4ed1-82a2-f2ef67cd97a5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Boilermaker RoomUpdated</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2-870 - Sculpture/OrnamentalUpdated</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10/25/2022 8:15:04 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://connectedoffice-devicemanagement.azurewebsites.net/Zones/Edit/d554a358-e10f-4d98-8c93-62bd2d1c5d46</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://connectedoffice-devicemanagement.azurewebsites.net/Zones/Details/d554a358-e10f-4d98-8c93-62bd2d1c5d46</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://connectedoffice-devicemanagement.azurewebsites.net/Zones/Delete/d554a358-e10f-4d98-8c93-62bd2d1c5d46</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10/25/2022 8:14:53 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://connectedoffice-devicemanagement.azurewebsites.net/Zones/Edit/efca46e9-6b5b-4212-95fe-83cc86bef3ba</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://connectedoffice-devicemanagement.azurewebsites.net/Zones/Details/efca46e9-6b5b-4212-95fe-83cc86bef3ba</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://connectedoffice-devicemanagement.azurewebsites.net/Zones/Delete/efca46e9-6b5b-4212-95fe-83cc86bef3ba</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Safety OfficeUpdated</x:t>
+  </x:si>
+  <x:si>
+    <x:t>17-030 - BondUpdated</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10/25/2022 7:20:45 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://connectedoffice-devicemanagement.azurewebsites.net/Zones/Edit/4201f294-c200-4e75-b4ac-6a45151601c2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://connectedoffice-devicemanagement.azurewebsites.net/Zones/Details/4201f294-c200-4e75-b4ac-6a45151601c2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://connectedoffice-devicemanagement.azurewebsites.net/Zones/Delete/4201f294-c200-4e75-b4ac-6a45151601c2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Tile Setting BenchUpdated</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1-570 - Temporary ControlsUpdated</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10/25/2022 7:21:11 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://connectedoffice-devicemanagement.azurewebsites.net/Zones/Edit/d62a79c8-7968-40d0-bee9-943c0983752e</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://connectedoffice-devicemanagement.azurewebsites.net/Zones/Details/d62a79c8-7968-40d0-bee9-943c0983752e</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://connectedoffice-devicemanagement.azurewebsites.net/Zones/Delete/d62a79c8-7968-40d0-bee9-943c0983752e</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10/25/2022 7:20:40 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://connectedoffice-devicemanagement.azurewebsites.net/Zones/Edit/48dc1bd2-caf3-4282-a254-a674fafc42ec</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://connectedoffice-devicemanagement.azurewebsites.net/Zones/Details/48dc1bd2-caf3-4282-a254-a674fafc42ec</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://connectedoffice-devicemanagement.azurewebsites.net/Zones/Delete/48dc1bd2-caf3-4282-a254-a674fafc42ec</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Labor OfficeUpdated</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1-523 - Sanitary FacilitiesUpdated</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10/25/2022 7:21:01 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://connectedoffice-devicemanagement.azurewebsites.net/Zones/Edit/0dca1b39-6e01-423f-a734-c56f12ca7b53</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://connectedoffice-devicemanagement.azurewebsites.net/Zones/Details/0dca1b39-6e01-423f-a734-c56f12ca7b53</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://connectedoffice-devicemanagement.azurewebsites.net/Zones/Delete/0dca1b39-6e01-423f-a734-c56f12ca7b53</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Stucco Mason BuildingUpdated</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2-750 - Concrete Pads and WalksUpdated</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10/25/2022 7:20:51 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://connectedoffice-devicemanagement.azurewebsites.net/Zones/Edit/1122805a-abbc-4fc5-85c1-ef88b3cd4e2a</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://connectedoffice-devicemanagement.azurewebsites.net/Zones/Details/1122805a-abbc-4fc5-85c1-ef88b3cd4e2a</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://connectedoffice-devicemanagement.azurewebsites.net/Zones/Delete/1122805a-abbc-4fc5-85c1-ef88b3cd4e2a</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10/25/2022 7:20:30 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://connectedoffice-devicemanagement.azurewebsites.net/Zones/Edit/1c39bed7-abd1-4430-9551-ff464a872b2b</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://connectedoffice-devicemanagement.azurewebsites.net/Zones/Details/1c39bed7-abd1-4430-9551-ff464a872b2b</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://connectedoffice-devicemanagement.azurewebsites.net/Zones/Delete/1c39bed7-abd1-4430-9551-ff464a872b2b</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -441,6 +567,238 @@
         <x:v>10</x:v>
       </x:c>
     </x:row>
+    <x:row r="2" spans="1:16">
+      <x:c r="A2" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="E2" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="F2" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H2" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="I2" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="K2" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="L2" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:16">
+      <x:c r="A3" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="F3" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="H3" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="I3" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="K3" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="L3" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:16">
+      <x:c r="A4" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="F4" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="H4" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="I4" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="K4" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="L4" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:16">
+      <x:c r="A5" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="E5" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="F5" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="H5" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="I5" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="K5" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="L5" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:16">
+      <x:c r="A6" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="E6" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="F6" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="H6" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="I6" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="K6" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="L6" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:16">
+      <x:c r="A7" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="E7" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="F7" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="H7" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="I7" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="K7" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="L7" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:16">
+      <x:c r="A8" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="E8" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="F8" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="H8" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="I8" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="K8" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="L8" s="0" t="s">
+        <x:v>48</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:16">
+      <x:c r="A9" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C9" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="E9" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="F9" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="H9" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="I9" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="K9" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="L9" s="0" t="s">
+        <x:v>52</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>